<commit_message>
update PANELS materials for wet weight
</commit_message>
<xml_diff>
--- a/panels/final_spreadsheets/panels_data_entry_spreadsheet_marinegeo.xlsx
+++ b/panels/final_spreadsheets/panels_data_entry_spreadsheet_marinegeo.xlsx
@@ -256,16 +256,16 @@
     <t xml:space="preserve">species_list_notes</t>
   </si>
   <si>
-    <t xml:space="preserve">temperature_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature, measured with a probe or sonde, in degrees Celsius</t>
-  </si>
-  <si>
     <t xml:space="preserve">topdown_photos_notes</t>
   </si>
   <si>
     <t xml:space="preserve">topdown photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wet_weight_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The total wet mass of the entire community that was scrapped off of the panel</t>
   </si>
 </sst>
 </file>
@@ -1312,15 +1312,15 @@
         <v>71</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31">
@@ -1328,15 +1328,15 @@
         <v>73</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32">
@@ -1387,13 +1387,12 @@
     <col min="8" max="8" width="13.71" hidden="0" customWidth="1"/>
     <col min="9" max="9" width="16.71" hidden="0" customWidth="1"/>
     <col min="10" max="10" width="17.71" hidden="0" customWidth="1"/>
-    <col min="11" max="11" width="13.71" hidden="0" customWidth="1"/>
-    <col min="12" max="12" width="12.71" hidden="0" customWidth="1"/>
-    <col min="13" max="13" width="15.71" hidden="0" customWidth="1"/>
-    <col min="14" max="14" width="16.71" hidden="0" customWidth="1"/>
-    <col min="15" max="15" width="21.71" hidden="0" customWidth="1"/>
-    <col min="16" max="16" width="23.71" hidden="0" customWidth="1"/>
-    <col min="17" max="17" width="19.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="12.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="15.71" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="16.71" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="21.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="23.71" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="19.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1428,24 +1427,21 @@
         <v>23</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="12" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1480,7 +1476,7 @@
         <v>49</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1530,8 @@
     <col min="1" max="1" width="13.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="19.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="10.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="12.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="10.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1548,6 +1545,9 @@
         <v>36</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add PANELS protocol document
</commit_message>
<xml_diff>
--- a/panels/final_spreadsheets/panels_data_entry_spreadsheet_marinegeo.xlsx
+++ b/panels/final_spreadsheets/panels_data_entry_spreadsheet_marinegeo.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>definition</t>
   </si>
@@ -100,6 +100,27 @@
     <t xml:space="preserve">site metadata, topdown photos, 3D photos, eDNA, species list</t>
   </si>
   <si>
+    <t xml:space="preserve">community_wet_weight_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The total wet mass of the entire community that was scrapped off of the panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eDNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">container_and_community_weight_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The total weight of the community sample and the container</t>
+  </si>
+  <si>
+    <t xml:space="preserve">container_weight_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The weight of the container prior to adding the sample</t>
+  </si>
+  <si>
     <t xml:space="preserve">decimal_latitude</t>
   </si>
   <si>
@@ -142,9 +163,6 @@
     <t xml:space="preserve">eDNA_notes</t>
   </si>
   <si>
-    <t xml:space="preserve">eDNA</t>
-  </si>
-  <si>
     <t xml:space="preserve">identification_notes</t>
   </si>
   <si>
@@ -260,12 +278,6 @@
   </si>
   <si>
     <t xml:space="preserve">topdown photos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wet_weight_g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The total wet mass of the entire community that was scrapped off of the panel</t>
   </si>
 </sst>
 </file>
@@ -927,38 +939,34 @@
       <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>17</v>
@@ -966,23 +974,25 @@
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
@@ -993,36 +1003,38 @@
         <v>31</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>13</v>
@@ -1030,15 +1042,15 @@
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>13</v>
@@ -1046,15 +1058,15 @@
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>13</v>
@@ -1062,7 +1074,7 @@
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
@@ -1070,7 +1082,7 @@
         <v>40</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>13</v>
@@ -1078,7 +1090,7 @@
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16">
@@ -1094,7 +1106,7 @@
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
@@ -1110,7 +1122,7 @@
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
@@ -1126,15 +1138,15 @@
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>13</v>
@@ -1142,15 +1154,15 @@
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>13</v>
@@ -1158,31 +1170,31 @@
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>13</v>
@@ -1190,7 +1202,7 @@
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23">
@@ -1206,7 +1218,7 @@
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24">
@@ -1217,12 +1229,12 @@
         <v>61</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25">
@@ -1238,7 +1250,7 @@
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26">
@@ -1254,7 +1266,7 @@
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27">
@@ -1267,20 +1279,18 @@
       <c r="C27" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>68</v>
-      </c>
+      <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>13</v>
@@ -1288,7 +1298,7 @@
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29">
@@ -1296,7 +1306,7 @@
         <v>70</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>13</v>
@@ -1304,48 +1314,82 @@
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
+      <c r="A32" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1397,52 +1441,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1470,13 +1514,13 @@
         <v>15</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1504,10 +1548,10 @@
         <v>15</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>11</v>
@@ -1530,8 +1574,10 @@
     <col min="1" max="1" width="13.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="8.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="19.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="12.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="10.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="18.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="32.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="22.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="10.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1539,16 +1585,22 @@
         <v>15</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1579,22 +1631,22 @@
         <v>15</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>